<commit_message>
add create_cumulative_data change predict_income
</commit_message>
<xml_diff>
--- a/database/industries/felezat/fasmin/balancesheet/quarterly.xlsx
+++ b/database/industries/felezat/fasmin/balancesheet/quarterly.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\felezat\fasmin\balancesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\felezat\fasmin\balancesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A114726C-7064-422B-8C15-1E5F274EB073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="2748" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -37,6 +36,21 @@
     <t>دوره مالی</t>
   </si>
   <si>
+    <t>فصل دوم منتهی به 1399/06</t>
+  </si>
+  <si>
+    <t>فصل سوم منتهی به 1399/09</t>
+  </si>
+  <si>
+    <t>فصل چهارم منتهی به 1399/12</t>
+  </si>
+  <si>
+    <t>فصل اول منتهی به 1400/03</t>
+  </si>
+  <si>
+    <t>فصل دوم منتهی به 1400/06</t>
+  </si>
+  <si>
     <t>فصل سوم منتهی به 1400/09</t>
   </si>
   <si>
@@ -53,6 +67,21 @@
   </si>
   <si>
     <t>تاریخ انتشار</t>
+  </si>
+  <si>
+    <t>1399-10-15 (2)</t>
+  </si>
+  <si>
+    <t>1399-11-02</t>
+  </si>
+  <si>
+    <t>1401-04-21 (11)</t>
+  </si>
+  <si>
+    <t>1400-04-29</t>
+  </si>
+  <si>
+    <t>1400-10-09 (3)</t>
   </si>
   <si>
     <t>1400-11-24 (2)</t>
@@ -220,7 +249,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,7 +447,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -430,7 +459,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -477,23 +506,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -529,23 +541,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -697,21 +692,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="8" width="29" customWidth="1"/>
+    <col min="4" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="31" customWidth="1"/>
+    <col min="11" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -719,8 +716,13 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -730,8 +732,13 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -741,8 +748,13 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -750,8 +762,13 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="2:8" ht="40.799999999999997" x14ac:dyDescent="0.75">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -761,8 +778,13 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="2:8" ht="40.799999999999997" x14ac:dyDescent="0.75">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="2:13" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -772,8 +794,13 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -781,8 +808,13 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -802,29 +834,59 @@
       <c r="H8" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -832,10 +894,15 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -843,115 +910,195 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15">
+        <v>209795</v>
+      </c>
+      <c r="E12" s="15">
+        <v>134833</v>
+      </c>
+      <c r="F12" s="15">
+        <v>307408</v>
+      </c>
+      <c r="G12" s="15">
+        <v>499073</v>
+      </c>
+      <c r="H12" s="15">
+        <v>307636</v>
+      </c>
+      <c r="I12" s="15">
         <v>1933784</v>
       </c>
-      <c r="E12" s="15">
+      <c r="J12" s="15">
         <v>1825805</v>
       </c>
-      <c r="F12" s="15">
+      <c r="K12" s="15">
         <v>4724509</v>
       </c>
-      <c r="G12" s="15">
+      <c r="L12" s="15">
         <v>2043105</v>
       </c>
-      <c r="H12" s="15">
+      <c r="M12" s="15">
         <v>1740977</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11">
+        <v>843071</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2292900</v>
+      </c>
+      <c r="F13" s="11">
+        <v>743071</v>
+      </c>
+      <c r="G13" s="11">
+        <v>743071</v>
+      </c>
+      <c r="H13" s="11">
+        <v>743071</v>
+      </c>
+      <c r="I13" s="11">
         <v>742900</v>
       </c>
-      <c r="E13" s="11">
+      <c r="J13" s="11">
         <v>2743071</v>
       </c>
-      <c r="F13" s="11">
+      <c r="K13" s="11">
         <v>2743071</v>
       </c>
-      <c r="G13" s="11">
+      <c r="L13" s="11">
         <v>4088071</v>
       </c>
-      <c r="H13" s="11">
+      <c r="M13" s="11">
         <v>157900</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15">
+        <v>7933106</v>
+      </c>
+      <c r="E14" s="15">
+        <v>11697762</v>
+      </c>
+      <c r="F14" s="15">
+        <v>9914058</v>
+      </c>
+      <c r="G14" s="15">
+        <v>11407115</v>
+      </c>
+      <c r="H14" s="15">
+        <v>11627472</v>
+      </c>
+      <c r="I14" s="15">
         <v>11945335</v>
       </c>
-      <c r="E14" s="15">
+      <c r="J14" s="15">
         <v>18735275</v>
       </c>
-      <c r="F14" s="15">
+      <c r="K14" s="15">
         <v>16610790</v>
       </c>
-      <c r="G14" s="15">
+      <c r="L14" s="15">
         <v>22266278</v>
       </c>
-      <c r="H14" s="15">
+      <c r="M14" s="15">
         <v>29595049</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11">
+        <v>7573117</v>
+      </c>
+      <c r="E15" s="11">
+        <v>8745336</v>
+      </c>
+      <c r="F15" s="11">
+        <v>10828334</v>
+      </c>
+      <c r="G15" s="11">
+        <v>14264419</v>
+      </c>
+      <c r="H15" s="11">
+        <v>17627591</v>
+      </c>
+      <c r="I15" s="11">
         <v>20475783</v>
       </c>
-      <c r="E15" s="11">
+      <c r="J15" s="11">
         <v>22962356</v>
       </c>
-      <c r="F15" s="11">
+      <c r="K15" s="11">
         <v>25452002</v>
       </c>
-      <c r="G15" s="11">
+      <c r="L15" s="11">
         <v>31075353</v>
       </c>
-      <c r="H15" s="11">
+      <c r="M15" s="11">
         <v>31709954</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15">
+        <v>283807</v>
+      </c>
+      <c r="E16" s="15">
+        <v>657432</v>
+      </c>
+      <c r="F16" s="15">
+        <v>947517</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1731997</v>
+      </c>
+      <c r="H16" s="15">
+        <v>880800</v>
+      </c>
+      <c r="I16" s="15">
         <v>954557</v>
       </c>
-      <c r="E16" s="15">
+      <c r="J16" s="15">
         <v>101032</v>
       </c>
-      <c r="F16" s="15">
+      <c r="K16" s="15">
         <v>95489</v>
       </c>
-      <c r="G16" s="15">
+      <c r="L16" s="15">
         <v>122589</v>
       </c>
-      <c r="H16" s="15">
+      <c r="M16" s="15">
         <v>4222386</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11">
@@ -969,31 +1116,61 @@
       <c r="H17" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17">
+        <v>16842896</v>
+      </c>
+      <c r="E18" s="17">
+        <v>23528263</v>
+      </c>
+      <c r="F18" s="17">
+        <v>22740388</v>
+      </c>
+      <c r="G18" s="17">
+        <v>28645675</v>
+      </c>
+      <c r="H18" s="17">
+        <v>31186570</v>
+      </c>
+      <c r="I18" s="17">
         <v>36052359</v>
       </c>
-      <c r="E18" s="17">
+      <c r="J18" s="17">
         <v>46367539</v>
       </c>
-      <c r="F18" s="17">
+      <c r="K18" s="17">
         <v>49625861</v>
       </c>
-      <c r="G18" s="17">
+      <c r="L18" s="17">
         <v>59595396</v>
       </c>
-      <c r="H18" s="17">
+      <c r="M18" s="17">
         <v>67426266</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11">
@@ -1011,31 +1188,61 @@
       <c r="H19" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="11">
+        <v>0</v>
+      </c>
+      <c r="J19" s="11">
+        <v>0</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
+      <c r="M19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15">
+        <v>662875</v>
+      </c>
+      <c r="E20" s="15">
+        <v>665033</v>
+      </c>
+      <c r="F20" s="15">
+        <v>665262</v>
+      </c>
+      <c r="G20" s="15">
+        <v>665262</v>
+      </c>
+      <c r="H20" s="15">
+        <v>665262</v>
+      </c>
+      <c r="I20" s="15">
         <v>665433</v>
       </c>
-      <c r="E20" s="15">
+      <c r="J20" s="15">
         <v>665628</v>
       </c>
-      <c r="F20" s="15">
+      <c r="K20" s="15">
         <v>665628</v>
       </c>
-      <c r="G20" s="15">
+      <c r="L20" s="15">
         <v>666548</v>
       </c>
-      <c r="H20" s="15">
+      <c r="M20" s="15">
         <v>665780</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11">
@@ -1053,80 +1260,140 @@
       <c r="H21" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
+        <v>0</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0</v>
+      </c>
+      <c r="M21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15">
+        <v>1765290</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1788773</v>
+      </c>
+      <c r="F22" s="15">
+        <v>1904236</v>
+      </c>
+      <c r="G22" s="15">
+        <v>1879043</v>
+      </c>
+      <c r="H22" s="15">
+        <v>1961084</v>
+      </c>
+      <c r="I22" s="15">
         <v>1911465</v>
       </c>
-      <c r="E22" s="15">
+      <c r="J22" s="15">
         <v>2142842</v>
       </c>
-      <c r="F22" s="15">
+      <c r="K22" s="15">
         <v>2135513</v>
       </c>
-      <c r="G22" s="15">
+      <c r="L22" s="15">
         <v>2131912</v>
       </c>
-      <c r="H22" s="15">
+      <c r="M22" s="15">
         <v>2037586</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11">
+        <v>40793</v>
+      </c>
+      <c r="E23" s="11">
+        <v>40716</v>
+      </c>
+      <c r="F23" s="11">
+        <v>40623</v>
+      </c>
+      <c r="G23" s="11">
+        <v>40098</v>
+      </c>
+      <c r="H23" s="11">
+        <v>40405</v>
+      </c>
+      <c r="I23" s="11">
         <v>40406</v>
       </c>
-      <c r="E23" s="11">
+      <c r="J23" s="11">
         <v>61822</v>
       </c>
-      <c r="F23" s="11">
+      <c r="K23" s="11">
         <v>59248</v>
       </c>
-      <c r="G23" s="11">
+      <c r="L23" s="11">
         <v>61242</v>
       </c>
-      <c r="H23" s="11">
+      <c r="M23" s="11">
         <v>45388</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11">
-        <v>0</v>
+        <v>1369</v>
       </c>
       <c r="E25" s="11">
-        <v>0</v>
+        <v>1369</v>
       </c>
       <c r="F25" s="11">
         <v>0</v>
@@ -1137,52 +1404,97 @@
       <c r="H25" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
+        <v>0</v>
+      </c>
+      <c r="K25" s="11">
+        <v>0</v>
+      </c>
+      <c r="L25" s="11">
+        <v>0</v>
+      </c>
+      <c r="M25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17">
+        <v>2470327</v>
+      </c>
+      <c r="E26" s="17">
+        <v>2495891</v>
+      </c>
+      <c r="F26" s="17">
+        <v>2610121</v>
+      </c>
+      <c r="G26" s="17">
+        <v>2584403</v>
+      </c>
+      <c r="H26" s="17">
+        <v>2666751</v>
+      </c>
+      <c r="I26" s="17">
         <v>2617304</v>
       </c>
-      <c r="E26" s="17">
+      <c r="J26" s="17">
         <v>2870292</v>
       </c>
-      <c r="F26" s="17">
+      <c r="K26" s="17">
         <v>2860389</v>
       </c>
-      <c r="G26" s="17">
+      <c r="L26" s="17">
         <v>2859702</v>
       </c>
-      <c r="H26" s="17">
+      <c r="M26" s="17">
         <v>2748754</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19">
+        <v>19313223</v>
+      </c>
+      <c r="E27" s="19">
+        <v>26024154</v>
+      </c>
+      <c r="F27" s="19">
+        <v>25350509</v>
+      </c>
+      <c r="G27" s="19">
+        <v>31230078</v>
+      </c>
+      <c r="H27" s="19">
+        <v>33853321</v>
+      </c>
+      <c r="I27" s="19">
         <v>38669663</v>
       </c>
-      <c r="E27" s="19">
+      <c r="J27" s="19">
         <v>49237831</v>
       </c>
-      <c r="F27" s="19">
+      <c r="K27" s="19">
         <v>52486250</v>
       </c>
-      <c r="G27" s="19">
+      <c r="L27" s="19">
         <v>62455098</v>
       </c>
-      <c r="H27" s="19">
+      <c r="M27" s="19">
         <v>70175020</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1190,136 +1502,231 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15">
+        <v>3503650</v>
+      </c>
+      <c r="E29" s="15">
+        <v>5721258</v>
+      </c>
+      <c r="F29" s="15">
+        <v>2464518</v>
+      </c>
+      <c r="G29" s="15">
+        <v>5500799</v>
+      </c>
+      <c r="H29" s="15">
+        <v>4443028</v>
+      </c>
+      <c r="I29" s="15">
         <v>3925462</v>
       </c>
-      <c r="E29" s="15">
+      <c r="J29" s="15">
         <v>6270787</v>
       </c>
-      <c r="F29" s="15">
+      <c r="K29" s="15">
         <v>3702134</v>
       </c>
-      <c r="G29" s="15">
+      <c r="L29" s="15">
         <v>7499795</v>
       </c>
-      <c r="H29" s="15">
+      <c r="M29" s="15">
         <v>13191985</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15">
-        <v>0</v>
+        <v>36378</v>
       </c>
       <c r="E31" s="15">
+        <v>2975</v>
+      </c>
+      <c r="F31" s="15">
+        <v>695714</v>
+      </c>
+      <c r="G31" s="15">
+        <v>1706</v>
+      </c>
+      <c r="H31" s="15">
+        <v>0</v>
+      </c>
+      <c r="I31" s="15">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15">
         <v>2151</v>
       </c>
-      <c r="F31" s="15">
+      <c r="K31" s="15">
         <v>1430</v>
       </c>
-      <c r="G31" s="15">
+      <c r="L31" s="15">
         <v>92366</v>
       </c>
-      <c r="H31" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="M31" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11">
+        <v>479844</v>
+      </c>
+      <c r="E32" s="11">
+        <v>587174</v>
+      </c>
+      <c r="F32" s="11">
+        <v>522698</v>
+      </c>
+      <c r="G32" s="11">
+        <v>761073</v>
+      </c>
+      <c r="H32" s="11">
+        <v>796710</v>
+      </c>
+      <c r="I32" s="11">
         <v>1039562</v>
       </c>
-      <c r="E32" s="11">
+      <c r="J32" s="11">
         <v>713851</v>
       </c>
-      <c r="F32" s="11">
-        <v>0</v>
-      </c>
-      <c r="G32" s="11">
+      <c r="K32" s="11">
+        <v>0</v>
+      </c>
+      <c r="L32" s="11">
         <v>1623251</v>
       </c>
-      <c r="H32" s="11">
+      <c r="M32" s="11">
         <v>1994354</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15">
+        <v>950401</v>
+      </c>
+      <c r="E33" s="15">
+        <v>921492</v>
+      </c>
+      <c r="F33" s="15">
+        <v>459378</v>
+      </c>
+      <c r="G33" s="15">
+        <v>254103</v>
+      </c>
+      <c r="H33" s="15">
+        <v>6170709</v>
+      </c>
+      <c r="I33" s="15">
         <v>6104356</v>
       </c>
-      <c r="E33" s="15">
+      <c r="J33" s="15">
         <v>4258490</v>
       </c>
-      <c r="F33" s="15">
+      <c r="K33" s="15">
         <v>3636188</v>
       </c>
-      <c r="G33" s="15">
+      <c r="L33" s="15">
         <v>15421220</v>
       </c>
-      <c r="H33" s="15">
+      <c r="M33" s="15">
         <v>11304651</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11">
-        <v>0</v>
+        <v>535760</v>
       </c>
       <c r="E34" s="11">
-        <v>0</v>
+        <v>503520</v>
       </c>
       <c r="F34" s="11">
         <v>0</v>
       </c>
       <c r="G34" s="11">
-        <v>0</v>
+        <v>381801</v>
       </c>
       <c r="H34" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="11">
+        <v>0</v>
+      </c>
+      <c r="J34" s="11">
+        <v>0</v>
+      </c>
+      <c r="K34" s="11">
+        <v>0</v>
+      </c>
+      <c r="L34" s="11">
+        <v>0</v>
+      </c>
+      <c r="M34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15">
@@ -1337,10 +1744,25 @@
       <c r="H35" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="15">
+        <v>0</v>
+      </c>
+      <c r="J35" s="15">
+        <v>0</v>
+      </c>
+      <c r="K35" s="15">
+        <v>0</v>
+      </c>
+      <c r="L35" s="15">
+        <v>0</v>
+      </c>
+      <c r="M35" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11">
@@ -1358,31 +1780,61 @@
       <c r="H36" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="11">
+        <v>0</v>
+      </c>
+      <c r="J36" s="11">
+        <v>0</v>
+      </c>
+      <c r="K36" s="11">
+        <v>0</v>
+      </c>
+      <c r="L36" s="11">
+        <v>0</v>
+      </c>
+      <c r="M36" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17">
+        <v>5506033</v>
+      </c>
+      <c r="E37" s="17">
+        <v>7736419</v>
+      </c>
+      <c r="F37" s="17">
+        <v>4142308</v>
+      </c>
+      <c r="G37" s="17">
+        <v>6899482</v>
+      </c>
+      <c r="H37" s="17">
+        <v>11410447</v>
+      </c>
+      <c r="I37" s="17">
         <v>11069380</v>
       </c>
-      <c r="E37" s="17">
+      <c r="J37" s="17">
         <v>11245279</v>
       </c>
-      <c r="F37" s="17">
+      <c r="K37" s="17">
         <v>7339752</v>
       </c>
-      <c r="G37" s="17">
+      <c r="L37" s="17">
         <v>24636632</v>
       </c>
-      <c r="H37" s="17">
+      <c r="M37" s="17">
         <v>26490990</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11">
@@ -1400,31 +1852,61 @@
       <c r="H38" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="11">
+        <v>0</v>
+      </c>
+      <c r="J38" s="11">
+        <v>0</v>
+      </c>
+      <c r="K38" s="11">
+        <v>0</v>
+      </c>
+      <c r="L38" s="11">
+        <v>0</v>
+      </c>
+      <c r="M38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11">
@@ -1442,73 +1924,133 @@
       <c r="H40" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="11">
+        <v>0</v>
+      </c>
+      <c r="J40" s="11">
+        <v>0</v>
+      </c>
+      <c r="K40" s="11">
+        <v>0</v>
+      </c>
+      <c r="L40" s="11">
+        <v>0</v>
+      </c>
+      <c r="M40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15">
+        <v>368495</v>
+      </c>
+      <c r="E41" s="15">
+        <v>372747</v>
+      </c>
+      <c r="F41" s="15">
+        <v>362307</v>
+      </c>
+      <c r="G41" s="15">
+        <v>384935</v>
+      </c>
+      <c r="H41" s="15">
+        <v>504541</v>
+      </c>
+      <c r="I41" s="15">
         <v>494466</v>
       </c>
-      <c r="E41" s="15">
+      <c r="J41" s="15">
         <v>490470</v>
       </c>
-      <c r="F41" s="15">
+      <c r="K41" s="15">
         <v>661135</v>
       </c>
-      <c r="G41" s="15">
+      <c r="L41" s="15">
         <v>777424</v>
       </c>
-      <c r="H41" s="15">
+      <c r="M41" s="15">
         <v>765762</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="18" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19">
+        <v>368495</v>
+      </c>
+      <c r="E42" s="19">
+        <v>372747</v>
+      </c>
+      <c r="F42" s="19">
+        <v>362307</v>
+      </c>
+      <c r="G42" s="19">
+        <v>384935</v>
+      </c>
+      <c r="H42" s="19">
+        <v>504541</v>
+      </c>
+      <c r="I42" s="19">
         <v>494466</v>
       </c>
-      <c r="E42" s="19">
+      <c r="J42" s="19">
         <v>490470</v>
       </c>
-      <c r="F42" s="19">
+      <c r="K42" s="19">
         <v>661135</v>
       </c>
-      <c r="G42" s="19">
+      <c r="L42" s="19">
         <v>777424</v>
       </c>
-      <c r="H42" s="19">
+      <c r="M42" s="19">
         <v>765762</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="16" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17">
+        <v>5874528</v>
+      </c>
+      <c r="E43" s="17">
+        <v>8109166</v>
+      </c>
+      <c r="F43" s="17">
+        <v>4504615</v>
+      </c>
+      <c r="G43" s="17">
+        <v>7284417</v>
+      </c>
+      <c r="H43" s="17">
+        <v>11914988</v>
+      </c>
+      <c r="I43" s="17">
         <v>11563846</v>
       </c>
-      <c r="E43" s="17">
+      <c r="J43" s="17">
         <v>11735749</v>
       </c>
-      <c r="F43" s="17">
+      <c r="K43" s="17">
         <v>8000887</v>
       </c>
-      <c r="G43" s="17">
+      <c r="L43" s="17">
         <v>25414056</v>
       </c>
-      <c r="H43" s="17">
+      <c r="M43" s="17">
         <v>27256752</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -1516,14 +2058,19 @@
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15">
-        <v>6000000</v>
+        <v>2000000</v>
       </c>
       <c r="E45" s="15">
         <v>6000000</v>
@@ -1537,10 +2084,25 @@
       <c r="H45" s="15">
         <v>6000000</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="15">
+        <v>6000000</v>
+      </c>
+      <c r="J45" s="15">
+        <v>6000000</v>
+      </c>
+      <c r="K45" s="15">
+        <v>6000000</v>
+      </c>
+      <c r="L45" s="15">
+        <v>6000000</v>
+      </c>
+      <c r="M45" s="15">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11">
@@ -1558,10 +2120,25 @@
       <c r="H46" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="11">
+        <v>0</v>
+      </c>
+      <c r="J46" s="11">
+        <v>0</v>
+      </c>
+      <c r="K46" s="11">
+        <v>0</v>
+      </c>
+      <c r="L46" s="11">
+        <v>0</v>
+      </c>
+      <c r="M46" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="15">
@@ -1579,31 +2156,61 @@
       <c r="H47" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="15">
+        <v>0</v>
+      </c>
+      <c r="J47" s="15">
+        <v>0</v>
+      </c>
+      <c r="K47" s="15">
+        <v>0</v>
+      </c>
+      <c r="L47" s="15">
+        <v>0</v>
+      </c>
+      <c r="M47" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="11">
+        <v>0</v>
+      </c>
+      <c r="E48" s="11">
+        <v>0</v>
+      </c>
+      <c r="F48" s="11">
+        <v>-196135</v>
+      </c>
+      <c r="G48" s="11">
+        <v>-196135</v>
+      </c>
+      <c r="H48" s="11">
         <v>-142769</v>
       </c>
-      <c r="E48" s="11">
+      <c r="I48" s="11">
+        <v>-142769</v>
+      </c>
+      <c r="J48" s="11">
         <v>-79958</v>
       </c>
-      <c r="F48" s="11">
+      <c r="K48" s="11">
         <v>-79958</v>
       </c>
-      <c r="G48" s="11">
+      <c r="L48" s="11">
         <v>-150511</v>
       </c>
-      <c r="H48" s="11">
+      <c r="M48" s="11">
         <v>-79958</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="15">
@@ -1613,25 +2220,40 @@
         <v>0</v>
       </c>
       <c r="F49" s="15">
-        <v>0</v>
+        <v>3079</v>
       </c>
       <c r="G49" s="15">
-        <v>0</v>
+        <v>3079</v>
       </c>
       <c r="H49" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I49" s="15">
+        <v>0</v>
+      </c>
+      <c r="J49" s="15">
+        <v>0</v>
+      </c>
+      <c r="K49" s="15">
+        <v>0</v>
+      </c>
+      <c r="L49" s="15">
+        <v>0</v>
+      </c>
+      <c r="M49" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="11">
-        <v>600000</v>
+        <v>200000</v>
       </c>
       <c r="E50" s="11">
-        <v>600000</v>
+        <v>200000</v>
       </c>
       <c r="F50" s="11">
         <v>600000</v>
@@ -1642,14 +2264,29 @@
       <c r="H50" s="11">
         <v>600000</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I50" s="11">
+        <v>600000</v>
+      </c>
+      <c r="J50" s="11">
+        <v>600000</v>
+      </c>
+      <c r="K50" s="11">
+        <v>600000</v>
+      </c>
+      <c r="L50" s="11">
+        <v>600000</v>
+      </c>
+      <c r="M50" s="11">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15">
-        <v>0</v>
+        <v>750000</v>
       </c>
       <c r="E51" s="15">
         <v>0</v>
@@ -1663,31 +2300,61 @@
       <c r="H51" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I51" s="15">
+        <v>0</v>
+      </c>
+      <c r="J51" s="15">
+        <v>0</v>
+      </c>
+      <c r="K51" s="15">
+        <v>0</v>
+      </c>
+      <c r="L51" s="15">
+        <v>0</v>
+      </c>
+      <c r="M51" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15">
@@ -1705,31 +2372,61 @@
       <c r="H53" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I53" s="15">
+        <v>0</v>
+      </c>
+      <c r="J53" s="15">
+        <v>0</v>
+      </c>
+      <c r="K53" s="15">
+        <v>0</v>
+      </c>
+      <c r="L53" s="15">
+        <v>0</v>
+      </c>
+      <c r="M53" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L54" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M54" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C55" s="15"/>
       <c r="D55" s="15">
@@ -1747,71 +2444,131 @@
       <c r="H55" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I55" s="15">
+        <v>0</v>
+      </c>
+      <c r="J55" s="15">
+        <v>0</v>
+      </c>
+      <c r="K55" s="15">
+        <v>0</v>
+      </c>
+      <c r="L55" s="15">
+        <v>0</v>
+      </c>
+      <c r="M55" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11">
+        <v>10488695</v>
+      </c>
+      <c r="E56" s="11">
+        <v>11714988</v>
+      </c>
+      <c r="F56" s="11">
+        <v>14438950</v>
+      </c>
+      <c r="G56" s="11">
+        <v>17538717</v>
+      </c>
+      <c r="H56" s="11">
+        <v>15481102</v>
+      </c>
+      <c r="I56" s="11">
         <v>20648586</v>
       </c>
-      <c r="E56" s="11">
+      <c r="J56" s="11">
         <v>30982040</v>
       </c>
-      <c r="F56" s="11">
+      <c r="K56" s="11">
         <v>37965321</v>
       </c>
-      <c r="G56" s="11">
+      <c r="L56" s="11">
         <v>30591553</v>
       </c>
-      <c r="H56" s="11">
+      <c r="M56" s="11">
         <v>36398226</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17">
+        <v>13438695</v>
+      </c>
+      <c r="E57" s="17">
+        <v>17914988</v>
+      </c>
+      <c r="F57" s="17">
+        <v>20845894</v>
+      </c>
+      <c r="G57" s="17">
+        <v>23945661</v>
+      </c>
+      <c r="H57" s="17">
+        <v>21938333</v>
+      </c>
+      <c r="I57" s="17">
         <v>27105817</v>
       </c>
-      <c r="E57" s="17">
+      <c r="J57" s="17">
         <v>37502082</v>
       </c>
-      <c r="F57" s="17">
+      <c r="K57" s="17">
         <v>44485363</v>
       </c>
-      <c r="G57" s="17">
+      <c r="L57" s="17">
         <v>37041042</v>
       </c>
-      <c r="H57" s="17">
+      <c r="M57" s="17">
         <v>42918268</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19">
+        <v>19313223</v>
+      </c>
+      <c r="E58" s="19">
+        <v>26024154</v>
+      </c>
+      <c r="F58" s="19">
+        <v>25350509</v>
+      </c>
+      <c r="G58" s="19">
+        <v>31230078</v>
+      </c>
+      <c r="H58" s="19">
+        <v>33853321</v>
+      </c>
+      <c r="I58" s="19">
         <v>38669663</v>
       </c>
-      <c r="E58" s="19">
+      <c r="J58" s="19">
         <v>49237831</v>
       </c>
-      <c r="F58" s="19">
+      <c r="K58" s="19">
         <v>52486250</v>
       </c>
-      <c r="G58" s="19">
+      <c r="L58" s="19">
         <v>62455098</v>
       </c>
-      <c r="H58" s="19">
+      <c r="M58" s="19">
         <v>70175020</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1819,6 +2576,11 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>